<commit_message>
timetable : rename data
</commit_message>
<xml_diff>
--- a/data/itis_groups.xlsx
+++ b/data/itis_groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\никита\Desktop\ITIS-helper\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/PycharmProjects/ITIS-helper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF2A6C0-2BD4-4704-9D1D-4FA46BE6C9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B1587C-94B0-0745-AC7C-BFA57A025766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E90D954-B691-4FE3-8BFA-61EF305A4FA8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{7E90D954-B691-4FE3-8BFA-61EF305A4FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>11-041</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Магистры</t>
   </si>
 </sst>
 </file>
@@ -558,297 +564,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299FC8C8-AFD5-4BAC-8A04-34E7A49904C8}">
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49:C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>